<commit_message>
append text updated to "-"
</commit_message>
<xml_diff>
--- a/src/test/resources/todos_testdata.xlsx
+++ b/src/test/resources/todos_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Durga\eclipse-workspace\HybridSeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86919214-84E5-482B-89BB-441FE56FA9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3285CE8-FCFF-44AF-8DFA-E69758EBCDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{D26C3DE8-EFC6-42A1-99CC-6D60E92534A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D26C3DE8-EFC6-42A1-99CC-6D60E92534A2}"/>
   </bookViews>
   <sheets>
     <sheet name="ToDosTasks" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,10 @@
     <t>Automation</t>
   </si>
   <si>
-    <t>no amendment</t>
-  </si>
-  <si>
     <t>Append Text</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -157,6 +157,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,7 +498,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,8 +533,8 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,8 +547,8 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,8 +561,8 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,8 +575,8 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,8 +589,8 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,8 +617,8 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,8 +631,8 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,8 +645,8 @@
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,8 +659,8 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
+      <c r="D11" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>